<commit_message>
update cmd device check
</commit_message>
<xml_diff>
--- a/Doc/高级时钟项目计划排期.xlsx
+++ b/Doc/高级时钟项目计划排期.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\DesignProject\AdvancedClock\Advanced-Clock\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B724E7E-B2F6-4BC0-A847-8616ACE67698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AD9A20-7B57-4818-97BC-14003875F7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,6 +92,24 @@
   <si>
     <t>a、main函数初始化+函数调度搭建（包括线程或者轮询、状态机等，以及tcp和usb的代码移植）
 b、makefile重新移植</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成，可以正常usb和网络通信</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本周完成通讯协议的设计与实现（3.24）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">功能实现：
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1、usb 速度测试
+2、LCD屏显示</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -450,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -508,7 +526,9 @@
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -521,52 +541,58 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>13</v>
+      <c r="B5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
@@ -602,9 +628,16 @@
       <c r="A12" s="2">
         <v>10</v>
       </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="2"/>
@@ -628,7 +661,10 @@
       <c r="A20" s="2"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
fix show err in net recv msg
</commit_message>
<xml_diff>
--- a/Doc/高级时钟项目计划排期.xlsx
+++ b/Doc/高级时钟项目计划排期.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\DesignProject\AdvancedClock\Advanced-Clock\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10AD9A20-7B57-4818-97BC-14003875F7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9EF45B-71CB-4D48-862D-8257C672571D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -110,6 +110,11 @@
   <si>
     <t>1、usb 速度测试
 2、LCD屏显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2024//03//25
+未完成，数据的接收和通讯协议的设计与编码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -471,7 +476,7 @@
   <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -531,7 +536,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -544,7 +549,9 @@
       <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>